<commit_message>
Refatoração da arquitetura do projeto
</commit_message>
<xml_diff>
--- a/clubFerias2/relatorios/Tempo de Uso por socio e categoria.xlsx
+++ b/clubFerias2/relatorios/Tempo de Uso por socio e categoria.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Socio</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>Relaxamento</t>
+  </si>
+  <si>
+    <t>Lazer</t>
   </si>
   <si>
     <t>Larissa Costa</t>
@@ -165,103 +168,127 @@
       <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E4" t="s" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refatoração Relatorios e Dao
</commit_message>
<xml_diff>
--- a/clubFerias2/relatorios/Tempo de Uso por socio e categoria.xlsx
+++ b/clubFerias2/relatorios/Tempo de Uso por socio e categoria.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
   <si>
     <t>Socio</t>
   </si>
@@ -29,10 +29,13 @@
     <t>Lazer</t>
   </si>
   <si>
+    <t>teste update dois</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Larissa Costa</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Joao Oliveira</t>
@@ -194,7 +197,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>6</v>
@@ -208,10 +211,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="3">
         <v>9</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>6</v>
       </c>
       <c r="C4" t="s" s="3">
         <v>6</v>
@@ -228,13 +231,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>6</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s" s="2">
         <v>6</v>
@@ -242,16 +245,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="3">
         <v>12</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>14</v>
       </c>
       <c r="E6" t="s" s="3">
         <v>6</v>
@@ -259,16 +262,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s" s="2">
         <v>15</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>6</v>
       </c>
       <c r="E7" t="s" s="2">
         <v>6</v>
@@ -279,15 +282,32 @@
         <v>16</v>
       </c>
       <c r="B8" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="C8" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s" s="3">
+      <c r="B9" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>